<commit_message>
Put Fig. 9.2 graph on another tab in Excel dataset
</commit_message>
<xml_diff>
--- a/chapters/ch09-Agriculture/datasets/Crippa et al 2021.xlsx
+++ b/chapters/ch09-Agriculture/datasets/Crippa et al 2021.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MCBook2021/chapters/ch09-Agriculture/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB354B11-39F5-2149-9729-24FF4DAC73BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220A40ED-7F4D-4442-90C5-D130793124E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{AAAC4583-13F8-4BA6-A554-E1AF1AB4DF10}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" activeTab="1" xr2:uid="{AAAC4583-13F8-4BA6-A554-E1AF1AB4DF10}"/>
   </bookViews>
   <sheets>
     <sheet name="data to plot" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Example Fig 9.2" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="32">
   <si>
     <t>USA</t>
   </si>
@@ -126,6 +127,12 @@
   <si>
     <t>End of life</t>
   </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
 </sst>
 </file>
 
@@ -207,7 +214,1060 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Example Fig 9.2'!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Example Fig 9.2'!$B$1:$AA$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1990</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1991</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1992</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1994</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2015</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Example Fig 9.2'!$B$2:$AA$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1204318.9745279572</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1215304.1477781972</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1230277.5630280967</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1236362.8321400147</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1261297.3436580398</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1354317.0111360985</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1317049.7815788726</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1335589.3703790447</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1350463.1590383556</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1387250.9273415278</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1411974.3985074153</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1405724.3886126149</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1451605.2706954302</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1451411.154614025</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1556558.3512991644</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1539365.4273239055</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1547942.590909861</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1687205.657044196</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1517618.5532496856</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1489595.3810372555</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1500704.1025076192</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1533758.2636879049</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1448819.2755584966</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1440514.847391533</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1473350.7195375226</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1470151.883198106</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1DEA-C741-80BF-AD7B911E47B7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="827185648"/>
+        <c:axId val="827276064"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="827185648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="827276064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="827276064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="827185648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DC5DD56-2F4F-6E47-A53F-27C15D8A5E32}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -572,8 +1632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B7ED962-AC3B-43B2-B245-2A95288E342E}">
   <dimension ref="A1:AA9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1545,6 +2605,240 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B48074F-8BB6-B94A-AAAF-28A83A596B87}">
+  <dimension ref="A1:AA2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="X8" sqref="X8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1">
+        <f>'data to plot'!B1</f>
+        <v>1990</v>
+      </c>
+      <c r="C1">
+        <f>'data to plot'!C1</f>
+        <v>1991</v>
+      </c>
+      <c r="D1">
+        <f>'data to plot'!D1</f>
+        <v>1992</v>
+      </c>
+      <c r="E1">
+        <f>'data to plot'!E1</f>
+        <v>1993</v>
+      </c>
+      <c r="F1">
+        <f>'data to plot'!F1</f>
+        <v>1994</v>
+      </c>
+      <c r="G1">
+        <f>'data to plot'!G1</f>
+        <v>1995</v>
+      </c>
+      <c r="H1">
+        <f>'data to plot'!H1</f>
+        <v>1996</v>
+      </c>
+      <c r="I1">
+        <f>'data to plot'!I1</f>
+        <v>1997</v>
+      </c>
+      <c r="J1">
+        <f>'data to plot'!J1</f>
+        <v>1998</v>
+      </c>
+      <c r="K1">
+        <f>'data to plot'!K1</f>
+        <v>1999</v>
+      </c>
+      <c r="L1">
+        <f>'data to plot'!L1</f>
+        <v>2000</v>
+      </c>
+      <c r="M1">
+        <f>'data to plot'!M1</f>
+        <v>2001</v>
+      </c>
+      <c r="N1">
+        <f>'data to plot'!N1</f>
+        <v>2002</v>
+      </c>
+      <c r="O1">
+        <f>'data to plot'!O1</f>
+        <v>2003</v>
+      </c>
+      <c r="P1">
+        <f>'data to plot'!P1</f>
+        <v>2004</v>
+      </c>
+      <c r="Q1">
+        <f>'data to plot'!Q1</f>
+        <v>2005</v>
+      </c>
+      <c r="R1">
+        <f>'data to plot'!R1</f>
+        <v>2006</v>
+      </c>
+      <c r="S1">
+        <f>'data to plot'!S1</f>
+        <v>2007</v>
+      </c>
+      <c r="T1">
+        <f>'data to plot'!T1</f>
+        <v>2008</v>
+      </c>
+      <c r="U1">
+        <f>'data to plot'!U1</f>
+        <v>2009</v>
+      </c>
+      <c r="V1">
+        <f>'data to plot'!V1</f>
+        <v>2010</v>
+      </c>
+      <c r="W1">
+        <f>'data to plot'!W1</f>
+        <v>2011</v>
+      </c>
+      <c r="X1">
+        <f>'data to plot'!X1</f>
+        <v>2012</v>
+      </c>
+      <c r="Y1">
+        <f>'data to plot'!Y1</f>
+        <v>2013</v>
+      </c>
+      <c r="Z1">
+        <f>'data to plot'!Z1</f>
+        <v>2014</v>
+      </c>
+      <c r="AA1">
+        <f>'data to plot'!AA1</f>
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <f>SUM('data to plot'!B2:B9)</f>
+        <v>1204318.9745279572</v>
+      </c>
+      <c r="C2">
+        <f>SUM('data to plot'!C2:C9)</f>
+        <v>1215304.1477781972</v>
+      </c>
+      <c r="D2">
+        <f>SUM('data to plot'!D2:D9)</f>
+        <v>1230277.5630280967</v>
+      </c>
+      <c r="E2">
+        <f>SUM('data to plot'!E2:E9)</f>
+        <v>1236362.8321400147</v>
+      </c>
+      <c r="F2">
+        <f>SUM('data to plot'!F2:F9)</f>
+        <v>1261297.3436580398</v>
+      </c>
+      <c r="G2">
+        <f>SUM('data to plot'!G2:G9)</f>
+        <v>1354317.0111360985</v>
+      </c>
+      <c r="H2">
+        <f>SUM('data to plot'!H2:H9)</f>
+        <v>1317049.7815788726</v>
+      </c>
+      <c r="I2">
+        <f>SUM('data to plot'!I2:I9)</f>
+        <v>1335589.3703790447</v>
+      </c>
+      <c r="J2">
+        <f>SUM('data to plot'!J2:J9)</f>
+        <v>1350463.1590383556</v>
+      </c>
+      <c r="K2">
+        <f>SUM('data to plot'!K2:K9)</f>
+        <v>1387250.9273415278</v>
+      </c>
+      <c r="L2">
+        <f>SUM('data to plot'!L2:L9)</f>
+        <v>1411974.3985074153</v>
+      </c>
+      <c r="M2">
+        <f>SUM('data to plot'!M2:M9)</f>
+        <v>1405724.3886126149</v>
+      </c>
+      <c r="N2">
+        <f>SUM('data to plot'!N2:N9)</f>
+        <v>1451605.2706954302</v>
+      </c>
+      <c r="O2">
+        <f>SUM('data to plot'!O2:O9)</f>
+        <v>1451411.154614025</v>
+      </c>
+      <c r="P2">
+        <f>SUM('data to plot'!P2:P9)</f>
+        <v>1556558.3512991644</v>
+      </c>
+      <c r="Q2">
+        <f>SUM('data to plot'!Q2:Q9)</f>
+        <v>1539365.4273239055</v>
+      </c>
+      <c r="R2">
+        <f>SUM('data to plot'!R2:R9)</f>
+        <v>1547942.590909861</v>
+      </c>
+      <c r="S2">
+        <f>SUM('data to plot'!S2:S9)</f>
+        <v>1687205.657044196</v>
+      </c>
+      <c r="T2">
+        <f>SUM('data to plot'!T2:T9)</f>
+        <v>1517618.5532496856</v>
+      </c>
+      <c r="U2">
+        <f>SUM('data to plot'!U2:U9)</f>
+        <v>1489595.3810372555</v>
+      </c>
+      <c r="V2">
+        <f>SUM('data to plot'!V2:V9)</f>
+        <v>1500704.1025076192</v>
+      </c>
+      <c r="W2">
+        <f>SUM('data to plot'!W2:W9)</f>
+        <v>1533758.2636879049</v>
+      </c>
+      <c r="X2">
+        <f>SUM('data to plot'!X2:X9)</f>
+        <v>1448819.2755584966</v>
+      </c>
+      <c r="Y2">
+        <f>SUM('data to plot'!Y2:Y9)</f>
+        <v>1440514.847391533</v>
+      </c>
+      <c r="Z2">
+        <f>SUM('data to plot'!Z2:Z9)</f>
+        <v>1473350.7195375226</v>
+      </c>
+      <c r="AA2">
+        <f>SUM('data to plot'!AA2:AA9)</f>
+        <v>1470151.883198106</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDD3AF7D-CF7E-4824-94BA-9D121F97DF37}">
   <dimension ref="A1:AF35"/>
   <sheetViews>

</xml_diff>